<commit_message>
test file for pivot chart macro
</commit_message>
<xml_diff>
--- a/for Hector/son001.xlsx
+++ b/for Hector/son001.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="54">
   <si>
     <t>EA</t>
   </si>
@@ -106,12 +106,84 @@
   </si>
   <si>
     <t>04-2E530</t>
+  </si>
+  <si>
+    <t>L01</t>
+  </si>
+  <si>
+    <t>L02</t>
+  </si>
+  <si>
+    <t>L03</t>
+  </si>
+  <si>
+    <t>L04</t>
+  </si>
+  <si>
+    <t>L05</t>
+  </si>
+  <si>
+    <t>L06</t>
+  </si>
+  <si>
+    <t>L07</t>
+  </si>
+  <si>
+    <t>L08</t>
+  </si>
+  <si>
+    <t>L09</t>
+  </si>
+  <si>
+    <t>L10</t>
+  </si>
+  <si>
+    <t>L11</t>
+  </si>
+  <si>
+    <t>L12</t>
+  </si>
+  <si>
+    <t>L13</t>
+  </si>
+  <si>
+    <t>L14</t>
+  </si>
+  <si>
+    <t>L15</t>
+  </si>
+  <si>
+    <t>L16</t>
+  </si>
+  <si>
+    <t>L17</t>
+  </si>
+  <si>
+    <t>L18</t>
+  </si>
+  <si>
+    <t>L19</t>
+  </si>
+  <si>
+    <t>L20</t>
+  </si>
+  <si>
+    <t>L21</t>
+  </si>
+  <si>
+    <t>L22</t>
+  </si>
+  <si>
+    <t>L23</t>
+  </si>
+  <si>
+    <t>L24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -156,6 +228,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -234,6 +311,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -268,6 +346,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -443,16 +522,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H22"/>
+      <selection activeCell="J1" sqref="J1:AH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:34">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,8 +556,80 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -503,8 +654,23 @@
       <c r="H2" s="1">
         <v>1.07</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="J2">
+        <v>1992</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>1.07</v>
+      </c>
+      <c r="M2">
+        <v>39.53</v>
+      </c>
+      <c r="N2">
+        <v>7.9829999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -529,8 +695,17 @@
       <c r="H3" s="1">
         <v>7.9829999999999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="J3">
+        <v>1993</v>
+      </c>
+      <c r="K3">
+        <v>24.524000000000001</v>
+      </c>
+      <c r="L3">
+        <v>1.776</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -555,8 +730,17 @@
       <c r="H4" s="1">
         <v>1.776</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="J4">
+        <v>2000</v>
+      </c>
+      <c r="K4">
+        <v>50.6</v>
+      </c>
+      <c r="L4">
+        <v>7.9829999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -581,8 +765,53 @@
       <c r="H5" s="1">
         <v>7.9829999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="J5">
+        <v>2001</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>4.2859999999999996</v>
+      </c>
+      <c r="O5">
+        <v>23.013999999999999</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>2.5</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>5</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -607,8 +836,17 @@
       <c r="H6" s="1">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="J6">
+        <v>2004</v>
+      </c>
+      <c r="K6">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="L6">
+        <v>3.6150000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -633,8 +871,17 @@
       <c r="H7" s="1">
         <v>4.2859999999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="J7">
+        <v>2005</v>
+      </c>
+      <c r="K7">
+        <v>19.885000000000002</v>
+      </c>
+      <c r="L7">
+        <v>5.1150000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -659,8 +906,17 @@
       <c r="H8" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="J8">
+        <v>2006</v>
+      </c>
+      <c r="K8">
+        <v>50.6</v>
+      </c>
+      <c r="L8">
+        <v>7.9829999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -685,8 +941,23 @@
       <c r="H9" s="1">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="J9">
+        <v>2009</v>
+      </c>
+      <c r="K9">
+        <v>19.885000000000002</v>
+      </c>
+      <c r="L9">
+        <v>4.6189999999999998</v>
+      </c>
+      <c r="M9">
+        <v>26.096</v>
+      </c>
+      <c r="N9">
+        <v>7.9829999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -711,8 +982,29 @@
       <c r="H10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="J10">
+        <v>2010</v>
+      </c>
+      <c r="K10">
+        <v>16.2</v>
+      </c>
+      <c r="L10">
+        <v>0.1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0.1</v>
+      </c>
+      <c r="O10">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="P10">
+        <v>7.9829999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -737,8 +1029,23 @@
       <c r="H11" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="J11">
+        <v>2012</v>
+      </c>
+      <c r="K11">
+        <v>30.5</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -764,7 +1071,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:34">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -790,7 +1097,7 @@
         <v>3.6150000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:34">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -816,7 +1123,7 @@
         <v>5.1150000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:34">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -842,7 +1149,7 @@
         <v>7.9829999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:34">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1030,7 +1337,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1042,7 +1349,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
add more info to label, add more for lookup
</commit_message>
<xml_diff>
--- a/for Hector/son001.xlsx
+++ b/for Hector/son001.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="87">
   <si>
     <t>EA</t>
   </si>
@@ -178,6 +178,105 @@
   </si>
   <si>
     <t>L24</t>
+  </si>
+  <si>
+    <t>Beg PM</t>
+  </si>
+  <si>
+    <t>End PM</t>
+  </si>
+  <si>
+    <t>Beg PM:   10.000</t>
+  </si>
+  <si>
+    <t>End PM:   11.070</t>
+  </si>
+  <si>
+    <t>Beg PM:   50.600</t>
+  </si>
+  <si>
+    <t>End PM:   58.583</t>
+  </si>
+  <si>
+    <t>Beg PM:   24.524</t>
+  </si>
+  <si>
+    <t>End PM:   26.300</t>
+  </si>
+  <si>
+    <t>Beg PM:    0.000</t>
+  </si>
+  <si>
+    <t>End PM:    8.400</t>
+  </si>
+  <si>
+    <t>Beg PM:    8.200</t>
+  </si>
+  <si>
+    <t>End PM:   12.486</t>
+  </si>
+  <si>
+    <t>Beg PM:   35.500</t>
+  </si>
+  <si>
+    <t>End PM:   39.500</t>
+  </si>
+  <si>
+    <t>Beg PM:   39.500</t>
+  </si>
+  <si>
+    <t>End PM:   42.000</t>
+  </si>
+  <si>
+    <t>Beg PM:   42.000</t>
+  </si>
+  <si>
+    <t>End PM:   43.000</t>
+  </si>
+  <si>
+    <t>Beg PM:   43.000</t>
+  </si>
+  <si>
+    <t>End PM:   48.000</t>
+  </si>
+  <si>
+    <t>Beg PM:   48.000</t>
+  </si>
+  <si>
+    <t>End PM:   50.600</t>
+  </si>
+  <si>
+    <t>Beg PM:   16.100</t>
+  </si>
+  <si>
+    <t>End PM:   19.715</t>
+  </si>
+  <si>
+    <t>Beg PM:   19.885</t>
+  </si>
+  <si>
+    <t>End PM:   25.000</t>
+  </si>
+  <si>
+    <t>End PM:   24.504</t>
+  </si>
+  <si>
+    <t>Beg PM:   16.200</t>
+  </si>
+  <si>
+    <t>End PM:   16.300</t>
+  </si>
+  <si>
+    <t>Beg PM:   16.300</t>
+  </si>
+  <si>
+    <t>End PM:   16.400</t>
+  </si>
+  <si>
+    <t>Beg PM:   30.500</t>
+  </si>
+  <si>
+    <t>End PM:   35.500</t>
   </si>
 </sst>
 </file>
@@ -523,9 +622,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH22"/>
+  <dimension ref="A1:AH37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:AH11"/>
     </sheetView>
   </sheetViews>
@@ -1174,8 +1273,32 @@
       <c r="H16" s="1">
         <v>4.6189999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>4</v>
+      </c>
+      <c r="O16" t="s">
+        <v>54</v>
+      </c>
+      <c r="P16" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1200,8 +1323,32 @@
       <c r="H17" s="1">
         <v>7.9829999999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="J17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="1">
+        <v>1992</v>
+      </c>
+      <c r="O17" t="s">
+        <v>56</v>
+      </c>
+      <c r="P17" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1226,8 +1373,32 @@
       <c r="H18" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="J18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" s="1">
+        <v>1992</v>
+      </c>
+      <c r="O18" t="s">
+        <v>58</v>
+      </c>
+      <c r="P18" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>7.9829999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1252,8 +1423,32 @@
       <c r="H19" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="J19" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="1">
+        <v>1993</v>
+      </c>
+      <c r="O19" t="s">
+        <v>60</v>
+      </c>
+      <c r="P19" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>1.776</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1278,8 +1473,32 @@
       <c r="H20" s="1">
         <v>7.9829999999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="J20" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" s="1">
+        <v>2000</v>
+      </c>
+      <c r="O20" t="s">
+        <v>58</v>
+      </c>
+      <c r="P20" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>7.9829999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1304,8 +1523,32 @@
       <c r="H21" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="J21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" t="s">
+        <v>11</v>
+      </c>
+      <c r="N21" s="1">
+        <v>2001</v>
+      </c>
+      <c r="O21" t="s">
+        <v>62</v>
+      </c>
+      <c r="P21" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1328,6 +1571,420 @@
         <v>50.6</v>
       </c>
       <c r="H22" s="1">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J22" t="s">
+        <v>18</v>
+      </c>
+      <c r="K22" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" t="s">
+        <v>11</v>
+      </c>
+      <c r="N22" s="1">
+        <v>2001</v>
+      </c>
+      <c r="O22" t="s">
+        <v>64</v>
+      </c>
+      <c r="P22" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>4.2859999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="J23" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" t="s">
+        <v>11</v>
+      </c>
+      <c r="N23" s="1">
+        <v>2001</v>
+      </c>
+      <c r="O23" t="s">
+        <v>66</v>
+      </c>
+      <c r="P23" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="J24" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" t="s">
+        <v>11</v>
+      </c>
+      <c r="N24" s="1">
+        <v>2001</v>
+      </c>
+      <c r="O24" t="s">
+        <v>68</v>
+      </c>
+      <c r="P24" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="J25" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" t="s">
+        <v>11</v>
+      </c>
+      <c r="N25" s="1">
+        <v>2001</v>
+      </c>
+      <c r="O25" t="s">
+        <v>70</v>
+      </c>
+      <c r="P25" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="J26" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" t="s">
+        <v>17</v>
+      </c>
+      <c r="L26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" t="s">
+        <v>11</v>
+      </c>
+      <c r="N26" s="1">
+        <v>2001</v>
+      </c>
+      <c r="O26" t="s">
+        <v>72</v>
+      </c>
+      <c r="P26" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="J27" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" t="s">
+        <v>10</v>
+      </c>
+      <c r="M27" t="s">
+        <v>11</v>
+      </c>
+      <c r="N27" s="1">
+        <v>2001</v>
+      </c>
+      <c r="O27" t="s">
+        <v>74</v>
+      </c>
+      <c r="P27" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="J28" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" t="s">
+        <v>10</v>
+      </c>
+      <c r="M28" t="s">
+        <v>11</v>
+      </c>
+      <c r="N28" s="1">
+        <v>2004</v>
+      </c>
+      <c r="O28" t="s">
+        <v>76</v>
+      </c>
+      <c r="P28" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>3.6150000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="J29" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" t="s">
+        <v>10</v>
+      </c>
+      <c r="M29" t="s">
+        <v>11</v>
+      </c>
+      <c r="N29" s="1">
+        <v>2005</v>
+      </c>
+      <c r="O29" t="s">
+        <v>78</v>
+      </c>
+      <c r="P29" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>5.1150000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="J30" t="s">
+        <v>24</v>
+      </c>
+      <c r="K30" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" t="s">
+        <v>10</v>
+      </c>
+      <c r="M30" t="s">
+        <v>11</v>
+      </c>
+      <c r="N30" s="1">
+        <v>2006</v>
+      </c>
+      <c r="O30" t="s">
+        <v>58</v>
+      </c>
+      <c r="P30" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>7.9829999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="J31" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" t="s">
+        <v>9</v>
+      </c>
+      <c r="L31" t="s">
+        <v>10</v>
+      </c>
+      <c r="M31" t="s">
+        <v>11</v>
+      </c>
+      <c r="N31" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O31" t="s">
+        <v>78</v>
+      </c>
+      <c r="P31" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>4.6189999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="J32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K32" t="s">
+        <v>23</v>
+      </c>
+      <c r="L32" t="s">
+        <v>10</v>
+      </c>
+      <c r="M32" t="s">
+        <v>11</v>
+      </c>
+      <c r="N32" s="1">
+        <v>2009</v>
+      </c>
+      <c r="O32" t="s">
+        <v>58</v>
+      </c>
+      <c r="P32" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>7.9829999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="10:17">
+      <c r="J33" t="s">
+        <v>27</v>
+      </c>
+      <c r="K33" t="s">
+        <v>17</v>
+      </c>
+      <c r="L33" t="s">
+        <v>10</v>
+      </c>
+      <c r="M33" t="s">
+        <v>11</v>
+      </c>
+      <c r="N33" s="1">
+        <v>2010</v>
+      </c>
+      <c r="O33" t="s">
+        <v>81</v>
+      </c>
+      <c r="P33" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="10:17">
+      <c r="J34" t="s">
+        <v>27</v>
+      </c>
+      <c r="K34" t="s">
+        <v>17</v>
+      </c>
+      <c r="L34" t="s">
+        <v>10</v>
+      </c>
+      <c r="M34" t="s">
+        <v>11</v>
+      </c>
+      <c r="N34" s="1">
+        <v>2010</v>
+      </c>
+      <c r="O34" t="s">
+        <v>83</v>
+      </c>
+      <c r="P34" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" spans="10:17">
+      <c r="J35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" t="s">
+        <v>9</v>
+      </c>
+      <c r="L35" t="s">
+        <v>10</v>
+      </c>
+      <c r="M35" t="s">
+        <v>11</v>
+      </c>
+      <c r="N35" s="1">
+        <v>2010</v>
+      </c>
+      <c r="O35" t="s">
+        <v>58</v>
+      </c>
+      <c r="P35" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>7.9829999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="10:17">
+      <c r="J36" t="s">
+        <v>29</v>
+      </c>
+      <c r="K36" t="s">
+        <v>23</v>
+      </c>
+      <c r="L36" t="s">
+        <v>10</v>
+      </c>
+      <c r="M36" t="s">
+        <v>11</v>
+      </c>
+      <c r="N36" s="1">
+        <v>2012</v>
+      </c>
+      <c r="O36" t="s">
+        <v>85</v>
+      </c>
+      <c r="P36" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="10:17">
+      <c r="J37" t="s">
+        <v>29</v>
+      </c>
+      <c r="K37" t="s">
+        <v>9</v>
+      </c>
+      <c r="L37" t="s">
+        <v>10</v>
+      </c>
+      <c r="M37" t="s">
+        <v>11</v>
+      </c>
+      <c r="N37" s="1">
+        <v>2012</v>
+      </c>
+      <c r="O37" t="s">
+        <v>85</v>
+      </c>
+      <c r="P37" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q37" s="1">
         <v>20.100000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
job killing template, gantt chart for D4 Route 001
D4 reports, start to add more filters to the templates, prepare raw data
for the gantt chart requested by Tom. differentiate left and right
directions.
</commit_message>
<xml_diff>
--- a/for Hector/son001.xlsx
+++ b/for Hector/son001.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -316,10 +316,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -330,6 +333,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -378,7 +384,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -413,7 +419,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -624,1367 +630,1390 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:AH11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="23" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="34" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:34">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:34">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2">
         <v>1992</v>
       </c>
-      <c r="F2" s="1">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="F2" s="2">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2">
         <v>11.07</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>1.07</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>1992</v>
       </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-      <c r="L2">
+      <c r="K2" s="1">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1">
         <v>1.07</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <v>39.53</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <v>7.9829999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:34">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2">
         <v>1992</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>50.6</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>58.582999999999998</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>7.9829999999999997</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>1993</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
         <v>24.524000000000001</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>1.776</v>
       </c>
     </row>
     <row r="4" spans="1:34">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2">
         <v>1993</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
         <v>24.524000000000001</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>26.3</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>1.776</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <v>2000</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="1">
         <v>50.6</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="1">
         <v>7.9829999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:34">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2">
         <v>2000</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
         <v>50.6</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>58.582999999999998</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <v>7.9829999999999997</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="1">
         <v>2001</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="1">
         <v>0</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1">
         <v>8.1999999999999993</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="1">
         <v>0</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="1">
         <v>4.2859999999999996</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="1">
         <v>23.013999999999999</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="1">
         <v>4</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="1">
         <v>0</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="1">
         <v>2.5</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="1">
         <v>0</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="1">
         <v>1</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="1">
         <v>0</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="1">
         <v>5</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="1">
         <v>0</v>
       </c>
-      <c r="X5">
+      <c r="X5" s="1">
         <v>2.6</v>
       </c>
     </row>
     <row r="6" spans="1:34">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2">
         <v>2001</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>2004</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="1">
         <v>16.100000000000001</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="1">
         <v>3.6150000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:34">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2">
         <v>2001</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>12.486000000000001</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <v>4.2859999999999996</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <v>2005</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="1">
         <v>19.885000000000002</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="1">
         <v>5.1150000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:34">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2">
         <v>2001</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2">
         <v>35.5</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <v>39.5</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <v>4</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <v>2006</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="1">
         <v>50.6</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="1">
         <v>7.9829999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:34">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2">
         <v>2001</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>39.5</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
         <v>42</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <v>2.5</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="1">
         <v>2009</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="1">
         <v>19.885000000000002</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="1">
         <v>4.6189999999999998</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="1">
         <v>26.096</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="1">
         <v>7.9829999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:34">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2">
         <v>2001</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
         <v>42</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <v>43</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="2">
         <v>1</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>2010</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="1">
         <v>16.2</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="1">
         <v>0.1</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="1">
         <v>0</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="1">
         <v>0.1</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="1">
         <v>34.200000000000003</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="1">
         <v>7.9829999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:34">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2">
         <v>2001</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2">
         <v>43</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <v>48</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <v>5</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>2012</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="1">
         <v>30.5</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="1">
         <v>5</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="1">
         <v>0</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="1">
         <v>15.1</v>
       </c>
     </row>
     <row r="12" spans="1:34">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2">
         <v>2001</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="2">
         <v>48</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
         <v>50.6</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <v>2.6</v>
       </c>
     </row>
     <row r="13" spans="1:34">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2">
         <v>2004</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="2">
         <v>16.100000000000001</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
         <v>19.715</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="2">
         <v>3.6150000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:34">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2">
         <v>2005</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="2">
         <v>19.885000000000002</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
         <v>25</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="2">
         <v>5.1150000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:34">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2">
         <v>2006</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="2">
         <v>50.6</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
         <v>58.582999999999998</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="2">
         <v>7.9829999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:34">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1">
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2">
         <v>2009</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="2">
         <v>19.885000000000002</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="2">
         <v>24.504000000000001</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="2">
         <v>4.6189999999999998</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2">
         <v>2009</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="2">
         <v>50.6</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="2">
         <v>58.582999999999998</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="2">
         <v>7.9829999999999997</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L17" t="s">
-        <v>10</v>
-      </c>
-      <c r="M17" t="s">
-        <v>11</v>
-      </c>
-      <c r="N17" s="1">
+      <c r="L17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="2">
         <v>1992</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="Q17" s="2">
         <v>1.07</v>
       </c>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2">
         <v>2010</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="2">
         <v>16.2</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="2">
         <v>16.3</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="2">
         <v>0.1</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L18" t="s">
-        <v>10</v>
-      </c>
-      <c r="M18" t="s">
-        <v>11</v>
-      </c>
-      <c r="N18" s="1">
+      <c r="L18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" s="2">
         <v>1992</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="Q18" s="2">
         <v>7.9829999999999997</v>
       </c>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="1">
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2">
         <v>2010</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="2">
         <v>16.3</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="2">
         <v>16.399999999999999</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="2">
         <v>0.1</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L19" t="s">
-        <v>10</v>
-      </c>
-      <c r="M19" t="s">
-        <v>11</v>
-      </c>
-      <c r="N19" s="1">
+      <c r="L19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="2">
         <v>1993</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="Q19" s="2">
         <v>1.776</v>
       </c>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1">
+      <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="2">
         <v>2010</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="2">
         <v>50.6</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="2">
         <v>58.582999999999998</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="2">
         <v>7.9829999999999997</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L20" t="s">
-        <v>10</v>
-      </c>
-      <c r="M20" t="s">
-        <v>11</v>
-      </c>
-      <c r="N20" s="1">
+      <c r="L20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" s="2">
         <v>2000</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="Q20" s="2">
         <v>7.9829999999999997</v>
       </c>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="2">
         <v>2012</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="2">
         <v>30.5</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="2">
         <v>35.5</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="2">
         <v>5</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L21" t="s">
-        <v>10</v>
-      </c>
-      <c r="M21" t="s">
-        <v>11</v>
-      </c>
-      <c r="N21" s="1">
+      <c r="L21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N21" s="2">
         <v>2001</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="Q21" s="2">
         <v>8.4</v>
       </c>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="2">
         <v>2012</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="2">
         <v>30.5</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="2">
         <v>50.6</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="2">
         <v>20.100000000000001</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L22" t="s">
-        <v>10</v>
-      </c>
-      <c r="M22" t="s">
-        <v>11</v>
-      </c>
-      <c r="N22" s="1">
+      <c r="L22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N22" s="2">
         <v>2001</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="Q22" s="2">
         <v>4.2859999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:17">
-      <c r="J23" t="s">
+      <c r="J23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L23" t="s">
-        <v>10</v>
-      </c>
-      <c r="M23" t="s">
-        <v>11</v>
-      </c>
-      <c r="N23" s="1">
+      <c r="L23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N23" s="2">
         <v>2001</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P23" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q23" s="1">
+      <c r="Q23" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:17">
-      <c r="J24" t="s">
+      <c r="J24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L24" t="s">
-        <v>10</v>
-      </c>
-      <c r="M24" t="s">
-        <v>11</v>
-      </c>
-      <c r="N24" s="1">
+      <c r="L24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N24" s="2">
         <v>2001</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O24" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q24" s="1">
+      <c r="Q24" s="2">
         <v>2.5</v>
       </c>
     </row>
     <row r="25" spans="1:17">
-      <c r="J25" t="s">
+      <c r="J25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L25" t="s">
-        <v>10</v>
-      </c>
-      <c r="M25" t="s">
-        <v>11</v>
-      </c>
-      <c r="N25" s="1">
+      <c r="L25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N25" s="2">
         <v>2001</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="Q25" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:17">
-      <c r="J26" t="s">
+      <c r="J26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L26" t="s">
-        <v>10</v>
-      </c>
-      <c r="M26" t="s">
-        <v>11</v>
-      </c>
-      <c r="N26" s="1">
+      <c r="L26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N26" s="2">
         <v>2001</v>
       </c>
-      <c r="O26" t="s">
+      <c r="O26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="P26" t="s">
+      <c r="P26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="Q26" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:17">
-      <c r="J27" t="s">
+      <c r="J27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L27" t="s">
-        <v>10</v>
-      </c>
-      <c r="M27" t="s">
-        <v>11</v>
-      </c>
-      <c r="N27" s="1">
+      <c r="L27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N27" s="2">
         <v>2001</v>
       </c>
-      <c r="O27" t="s">
+      <c r="O27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="P27" t="s">
+      <c r="P27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="Q27" s="2">
         <v>2.6</v>
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="J28" t="s">
+      <c r="J28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L28" t="s">
-        <v>10</v>
-      </c>
-      <c r="M28" t="s">
-        <v>11</v>
-      </c>
-      <c r="N28" s="1">
+      <c r="L28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N28" s="2">
         <v>2004</v>
       </c>
-      <c r="O28" t="s">
+      <c r="O28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="P28" t="s">
+      <c r="P28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="Q28" s="2">
         <v>3.6150000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="J29" t="s">
+      <c r="J29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L29" t="s">
-        <v>10</v>
-      </c>
-      <c r="M29" t="s">
-        <v>11</v>
-      </c>
-      <c r="N29" s="1">
+      <c r="L29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N29" s="2">
         <v>2005</v>
       </c>
-      <c r="O29" t="s">
+      <c r="O29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="P29" t="s">
+      <c r="P29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="Q29" s="2">
         <v>5.1150000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:17">
-      <c r="J30" t="s">
+      <c r="J30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L30" t="s">
-        <v>10</v>
-      </c>
-      <c r="M30" t="s">
-        <v>11</v>
-      </c>
-      <c r="N30" s="1">
+      <c r="L30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N30" s="2">
         <v>2006</v>
       </c>
-      <c r="O30" t="s">
+      <c r="O30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="P30" t="s">
+      <c r="P30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="Q30" s="2">
         <v>7.9829999999999997</v>
       </c>
     </row>
     <row r="31" spans="1:17">
-      <c r="J31" t="s">
+      <c r="J31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L31" t="s">
-        <v>10</v>
-      </c>
-      <c r="M31" t="s">
-        <v>11</v>
-      </c>
-      <c r="N31" s="1">
+      <c r="L31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N31" s="2">
         <v>2009</v>
       </c>
-      <c r="O31" t="s">
+      <c r="O31" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="P31" t="s">
+      <c r="P31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="Q31" s="2">
         <v>4.6189999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:17">
-      <c r="J32" t="s">
+      <c r="J32" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L32" t="s">
-        <v>10</v>
-      </c>
-      <c r="M32" t="s">
-        <v>11</v>
-      </c>
-      <c r="N32" s="1">
+      <c r="L32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N32" s="2">
         <v>2009</v>
       </c>
-      <c r="O32" t="s">
+      <c r="O32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="P32" t="s">
+      <c r="P32" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="Q32" s="2">
         <v>7.9829999999999997</v>
       </c>
     </row>
     <row r="33" spans="10:17">
-      <c r="J33" t="s">
+      <c r="J33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L33" t="s">
-        <v>10</v>
-      </c>
-      <c r="M33" t="s">
-        <v>11</v>
-      </c>
-      <c r="N33" s="1">
+      <c r="L33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N33" s="2">
         <v>2010</v>
       </c>
-      <c r="O33" t="s">
+      <c r="O33" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="P33" t="s">
+      <c r="P33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q33" s="1">
+      <c r="Q33" s="2">
         <v>0.1</v>
       </c>
     </row>
     <row r="34" spans="10:17">
-      <c r="J34" t="s">
+      <c r="J34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K34" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L34" t="s">
-        <v>10</v>
-      </c>
-      <c r="M34" t="s">
-        <v>11</v>
-      </c>
-      <c r="N34" s="1">
+      <c r="L34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N34" s="2">
         <v>2010</v>
       </c>
-      <c r="O34" t="s">
+      <c r="O34" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="P34" t="s">
+      <c r="P34" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Q34" s="1">
+      <c r="Q34" s="2">
         <v>0.1</v>
       </c>
     </row>
     <row r="35" spans="10:17">
-      <c r="J35" t="s">
+      <c r="J35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L35" t="s">
-        <v>10</v>
-      </c>
-      <c r="M35" t="s">
-        <v>11</v>
-      </c>
-      <c r="N35" s="1">
+      <c r="L35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N35" s="2">
         <v>2010</v>
       </c>
-      <c r="O35" t="s">
+      <c r="O35" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="P35" t="s">
+      <c r="P35" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Q35" s="1">
+      <c r="Q35" s="2">
         <v>7.9829999999999997</v>
       </c>
     </row>
     <row r="36" spans="10:17">
-      <c r="J36" t="s">
+      <c r="J36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K36" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L36" t="s">
-        <v>10</v>
-      </c>
-      <c r="M36" t="s">
-        <v>11</v>
-      </c>
-      <c r="N36" s="1">
+      <c r="L36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N36" s="2">
         <v>2012</v>
       </c>
-      <c r="O36" t="s">
+      <c r="O36" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="P36" t="s">
+      <c r="P36" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Q36" s="1">
+      <c r="Q36" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="10:17">
-      <c r="J37" t="s">
+      <c r="J37" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L37" t="s">
-        <v>10</v>
-      </c>
-      <c r="M37" t="s">
-        <v>11</v>
-      </c>
-      <c r="N37" s="1">
+      <c r="L37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N37" s="2">
         <v>2012</v>
       </c>
-      <c r="O37" t="s">
+      <c r="O37" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="P37" t="s">
+      <c r="P37" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q37" s="1">
+      <c r="Q37" s="2">
         <v>20.100000000000001</v>
       </c>
     </row>

</xml_diff>